<commit_message>
Sync configuration files between languages
</commit_message>
<xml_diff>
--- a/Config/EN/Assets.xlsx
+++ b/Config/EN/Assets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D796F9F-1BB2-44F9-9FC7-0897DDA9DFC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF833DDF-786F-462E-8FD8-6CD93866816A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Get" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="7">
   <si>
     <t>Organization Unit ID</t>
   </si>
@@ -112,7 +112,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="14">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -242,17 +242,6 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
@@ -287,22 +276,21 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:F101">
   <autoFilter ref="A1:F101" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="6">
-    <tableColumn id="6" xr3:uid="{C68BBEAC-7A58-41FB-BA92-351982A4DA1B}" name="Organization Unit ID" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Organization Unit Name" totalsRowFunction="count" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{C68BBEAC-7A58-41FB-BA92-351982A4DA1B}" name="Organization Unit ID" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Organization Unit Name" totalsRowFunction="count" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{96DFDB45-0B9C-4367-9B24-D26DAD7C70E7}" name="Asset ID"/>
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Asset Name" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Type"/>
-    <tableColumn id="7" xr3:uid="{A067D188-197D-4A79-82E6-8C9B8EDABB7C}" name="Value" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{A067D188-197D-4A79-82E6-8C9B8EDABB7C}" name="Value" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G102" totalsRowShown="0">
-  <autoFilter ref="A1:G102" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="7">
-    <tableColumn id="3" xr3:uid="{FBE28F8B-F662-4318-9C4E-E65DF490FD40}" name="Organization Unit ID" dataDxfId="11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F102" totalsRowShown="0">
+  <autoFilter ref="A1:F102" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="6">
     <tableColumn id="7" xr3:uid="{9F5282FE-6479-41B7-8672-34D0C5F6C8EE}" name="Organization Unit Name" dataDxfId="10"/>
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Asset Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Type"/>
@@ -608,7 +596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B90804-4CC2-4F3A-A5A0-B313E9BACDDF}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1158,7 +1146,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G102"/>
+  <dimension ref="A1:F102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1166,749 +1154,644 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.08984375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="38.26953125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.08984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.26953125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
+      <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+      <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="2"/>
+      <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+      <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+      <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
+      <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+      <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
+      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="E27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="E28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="E29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="E30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="E31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="E32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="E33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="E34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="1"/>
       <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="E35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="E36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="1"/>
       <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="E37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="1"/>
       <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="E38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="1"/>
       <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="E39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="1"/>
       <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="E40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="1"/>
       <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="E41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="1"/>
       <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="E42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="1"/>
       <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="E43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="1"/>
       <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="E44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="1"/>
       <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="E45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="1"/>
       <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="E46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="1"/>
       <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="E47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="1"/>
       <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="E48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="1"/>
       <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="E49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="1"/>
       <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="E50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="1"/>
       <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-      <c r="E51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="1"/>
       <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="E52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="1"/>
       <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-      <c r="E53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="1"/>
       <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="E54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="1"/>
       <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
-      <c r="E55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="1"/>
       <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="E56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="1"/>
       <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
-      <c r="E57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="1"/>
       <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="E58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="1"/>
       <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="E59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="1"/>
       <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
-      <c r="E60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="1"/>
       <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="2"/>
-      <c r="B61" s="2"/>
-      <c r="E61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="1"/>
       <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
-      <c r="E62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="1"/>
       <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="2"/>
-      <c r="B63" s="2"/>
-      <c r="E63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="1"/>
       <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="2"/>
-      <c r="B64" s="2"/>
-      <c r="E64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="1"/>
       <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="2"/>
-      <c r="B65" s="2"/>
-      <c r="E65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="1"/>
       <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
-      <c r="E66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="1"/>
       <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="2"/>
-      <c r="B67" s="2"/>
-      <c r="E67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="1"/>
       <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="2"/>
-      <c r="B68" s="2"/>
-      <c r="E68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="1"/>
       <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="2"/>
-      <c r="B69" s="2"/>
-      <c r="E69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="1"/>
       <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="2"/>
-      <c r="B70" s="2"/>
-      <c r="E70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="1"/>
       <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="2"/>
-      <c r="B71" s="2"/>
-      <c r="E71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="1"/>
       <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="2"/>
-      <c r="B72" s="2"/>
-      <c r="E72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="1"/>
       <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="2"/>
-      <c r="B73" s="2"/>
-      <c r="E73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="1"/>
       <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="2"/>
-      <c r="B74" s="2"/>
-      <c r="E74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="1"/>
       <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="2"/>
-      <c r="B75" s="2"/>
-      <c r="E75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="1"/>
       <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="2"/>
-      <c r="B76" s="2"/>
-      <c r="E76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="1"/>
       <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="2"/>
-      <c r="B77" s="2"/>
-      <c r="E77" s="2"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="1"/>
       <c r="F77" s="1"/>
-      <c r="G77" s="1"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="2"/>
-      <c r="B78" s="2"/>
-      <c r="E78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="1"/>
       <c r="F78" s="1"/>
-      <c r="G78" s="1"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="2"/>
-      <c r="B79" s="2"/>
-      <c r="E79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="1"/>
       <c r="F79" s="1"/>
-      <c r="G79" s="1"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="2"/>
-      <c r="B80" s="2"/>
-      <c r="E80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="1"/>
       <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" s="2"/>
-      <c r="B81" s="2"/>
-      <c r="E81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="1"/>
       <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" s="2"/>
-      <c r="B82" s="2"/>
-      <c r="E82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="1"/>
       <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="2"/>
-      <c r="B83" s="2"/>
-      <c r="E83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="1"/>
       <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" s="2"/>
-      <c r="B84" s="2"/>
-      <c r="E84" s="2"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="1"/>
       <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" s="2"/>
-      <c r="B85" s="2"/>
-      <c r="E85" s="2"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="1"/>
       <c r="F85" s="1"/>
-      <c r="G85" s="1"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" s="2"/>
-      <c r="B86" s="2"/>
-      <c r="E86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="1"/>
       <c r="F86" s="1"/>
-      <c r="G86" s="1"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="2"/>
-      <c r="B87" s="2"/>
-      <c r="E87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="1"/>
       <c r="F87" s="1"/>
-      <c r="G87" s="1"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="2"/>
-      <c r="B88" s="2"/>
-      <c r="E88" s="2"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="1"/>
       <c r="F88" s="1"/>
-      <c r="G88" s="1"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" s="2"/>
-      <c r="B89" s="2"/>
-      <c r="E89" s="2"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="1"/>
       <c r="F89" s="1"/>
-      <c r="G89" s="1"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" s="2"/>
-      <c r="B90" s="2"/>
-      <c r="E90" s="2"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="1"/>
       <c r="F90" s="1"/>
-      <c r="G90" s="1"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" s="2"/>
-      <c r="B91" s="2"/>
-      <c r="E91" s="2"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="1"/>
       <c r="F91" s="1"/>
-      <c r="G91" s="1"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" s="2"/>
-      <c r="B92" s="2"/>
-      <c r="E92" s="2"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="1"/>
       <c r="F92" s="1"/>
-      <c r="G92" s="1"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" s="2"/>
-      <c r="B93" s="2"/>
-      <c r="E93" s="2"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="1"/>
       <c r="F93" s="1"/>
-      <c r="G93" s="1"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" s="2"/>
-      <c r="B94" s="2"/>
-      <c r="E94" s="2"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="1"/>
       <c r="F94" s="1"/>
-      <c r="G94" s="1"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" s="2"/>
-      <c r="B95" s="2"/>
-      <c r="E95" s="2"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="1"/>
       <c r="F95" s="1"/>
-      <c r="G95" s="1"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" s="2"/>
-      <c r="B96" s="2"/>
-      <c r="E96" s="2"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="1"/>
       <c r="F96" s="1"/>
-      <c r="G96" s="1"/>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" s="2"/>
-      <c r="B97" s="2"/>
-      <c r="E97" s="2"/>
+      <c r="D97" s="2"/>
+      <c r="E97" s="1"/>
       <c r="F97" s="1"/>
-      <c r="G97" s="1"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" s="2"/>
-      <c r="B98" s="2"/>
-      <c r="E98" s="2"/>
+      <c r="D98" s="2"/>
+      <c r="E98" s="1"/>
       <c r="F98" s="1"/>
-      <c r="G98" s="1"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" s="2"/>
-      <c r="B99" s="2"/>
-      <c r="E99" s="2"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="1"/>
       <c r="F99" s="1"/>
-      <c r="G99" s="1"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" s="2"/>
-      <c r="B100" s="2"/>
-      <c r="E100" s="2"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="1"/>
       <c r="F100" s="1"/>
-      <c r="G100" s="1"/>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" s="2"/>
-      <c r="B101" s="2"/>
-      <c r="E101" s="2"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="1"/>
       <c r="F101" s="1"/>
-      <c r="G101" s="1"/>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="2"/>
-      <c r="B102" s="2"/>
-      <c r="E102" s="2"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="1"/>
       <c r="F102" s="1"/>
-      <c r="G102" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{F44B3D79-6E85-4752-80E5-E171C2D51A7E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{F44B3D79-6E85-4752-80E5-E171C2D51A7E}">
       <formula1>"Text,Bool,Integer,Credential"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1924,7 +1807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECF20293-3040-451C-BEA0-1DF5FCF14B01}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>